<commit_message>
Update .gitignore and hotels_list.csv/xlsx
</commit_message>
<xml_diff>
--- a/data/out/hotels_list.xlsx
+++ b/data/out/hotels_list.xlsx
@@ -468,7 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>US$1,130</t>
+          <t>US$1,116</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -490,27 +490,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Meliá Paris Vendôme</t>
+          <t>Sonder Le Frochot</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>US$1,828</t>
+          <t>US$682</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>529</t>
+          <t>724</t>
         </is>
       </c>
     </row>
@@ -544,17 +544,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Auberge de Jeunesse HI Paris Yves Robert</t>
+          <t>St Christopher's Inn Paris - Canal</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>US$127</t>
+          <t>US$86</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -564,46 +564,46 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5,517</t>
+          <t>6,519</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>St Christopher's Inn Paris - Canal</t>
+          <t>The People - Paris Nation</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>US$86</t>
+          <t>US$121</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6,519</t>
+          <t>6,122</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Beau M Paris</t>
+          <t>Hotel Relais Bosquet by Malone</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>US$138</t>
+          <t>US$924</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -618,51 +618,51 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1,149</t>
+          <t>1,068</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Motel One Paris-Porte Dorée</t>
+          <t>Hotel Armoni Paris</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>US$495</t>
+          <t>US$550</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>6,979</t>
+          <t>1,899</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>St Christopher's Inn Paris - Gare du Nord</t>
+          <t>Odalys City Paris XVII</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>US$95</t>
+          <t>US$571</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -672,213 +672,213 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>9,248</t>
+          <t>3,845</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>The People - Paris Nation</t>
+          <t>St Christopher's Inn Paris - Gare du Nord</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>US$121</t>
+          <t>US$95</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6,122</t>
+          <t>9,248</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hôtel Le Daum</t>
+          <t>Auberge de Jeunesse HI Paris Yves Robert</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>US$536</t>
+          <t>US$127</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>943</t>
+          <t>5,517</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>The People - Paris Bercy</t>
+          <t>Hotel The Playce by Happyculture</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>US$154</t>
+          <t>US$450</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>5,976</t>
+          <t>2,242</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>UCPA SPORT STATION HOSTEL PARIS</t>
+          <t>Le Regent Montmartre by Hiphophostels</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>US$113</t>
+          <t>US$99</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5,139</t>
+          <t>5,885</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hotel des Carmes by Malone</t>
+          <t>citizenM Paris Champs-Élysées</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>US$812</t>
+          <t>US$1,167</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Exceptional</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2,787</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ibis Paris Gare du Nord Château Landon 10ème</t>
+          <t>Motel One Paris-Porte Dorée</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>US$551</t>
+          <t>US$495</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>8.7</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4,930</t>
+          <t>6,979</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The People Paris Belleville</t>
+          <t>The People - Paris Bercy</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>US$130</t>
+          <t>US$143</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2,735</t>
+          <t>5,976</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Le Regent Montmartre by Hiphophostels</t>
+          <t>B&amp;B HOTEL Paris 17 Batignolles</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>US$99</t>
+          <t>US$506</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>7.9</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -888,105 +888,105 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5,885</t>
+          <t>12,198</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Generator Paris</t>
+          <t>Beau M Paris</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>US$103</t>
+          <t>US$138</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>8.7</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>9,523</t>
+          <t>1,149</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Alliance 3</t>
+          <t>Hôtel Cabane - Orso Hotels</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>US$424</t>
+          <t>US$528</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>983</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Hotel Relais Bosquet by Malone</t>
+          <t>Hôtel le 209 Paris Bercy</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>US$924</t>
+          <t>US$547</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1,068</t>
+          <t>3,245</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Maison Eugenie</t>
+          <t>Hôtel Le Daum</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>US$706</t>
+          <t>US$536</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -996,51 +996,51 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>943</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Austin's Saint Lazare Hotel</t>
+          <t>ibis Paris Gare du Nord Château Landon 10ème</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>US$720</t>
+          <t>US$551</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2,537</t>
+          <t>4,930</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MIJE MARAIS</t>
+          <t>Generator Paris</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>US$206</t>
+          <t>US$103</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1050,78 +1050,78 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>4,756</t>
+          <t>9,523</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ibis Paris Canal Saint Martin</t>
+          <t>Elysees Niel Hotel</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>US$511</t>
+          <t>US$510</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1,685</t>
+          <t>1,369</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Zoku Paris</t>
+          <t>Hôtel Belloy Saint Germain</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>US$675</t>
+          <t>US$776</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Wonderful</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>884</t>
+          <t>718</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Hôtel Cabane - Orso Hotels</t>
+          <t>Hotel Du Cadran</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>US$528</t>
+          <t>US$784</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1131,34 +1131,34 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>983</t>
+          <t>795</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Timhotel Opéra Blanche Fontaine</t>
+          <t>Hotel Monceau Wagram</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>US$624</t>
+          <t>US$599</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1,683</t>
+          <t>1,379</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update hotel prices and ratings in hotels_list.csv
</commit_message>
<xml_diff>
--- a/data/out/hotels_list.xlsx
+++ b/data/out/hotels_list.xlsx
@@ -517,17 +517,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>The People - Paris Marais</t>
+          <t>Hôtel Duo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>US$157</t>
+          <t>US$686</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -537,24 +537,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>6,609</t>
+          <t>850</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>St Christopher's Inn Paris - Canal</t>
+          <t>St Christopher's Inn Paris - Gare du Nord</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>US$86</t>
+          <t>US$95</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -564,78 +564,78 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>6,519</t>
+          <t>9,248</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>The People - Paris Nation</t>
+          <t>St Christopher's Inn Paris - Canal</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>US$121</t>
+          <t>US$86</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6,122</t>
+          <t>6,519</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hotel Relais Bosquet by Malone</t>
+          <t>Generator Paris</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>US$924</t>
+          <t>US$101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1,068</t>
+          <t>9,523</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hotel Armoni Paris</t>
+          <t>The People - Paris Nation</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>US$550</t>
+          <t>US$121</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -645,78 +645,78 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1,899</t>
+          <t>6,122</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Odalys City Paris XVII</t>
+          <t>The People - Paris Bercy</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>US$571</t>
+          <t>US$143</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3,845</t>
+          <t>5,976</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>St Christopher's Inn Paris - Gare du Nord</t>
+          <t>Hotel de L'Empereur by Malone</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>US$95</t>
+          <t>US$741</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.6</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>9,248</t>
+          <t>992</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Auberge de Jeunesse HI Paris Yves Robert</t>
+          <t>Le Regent Montmartre by Hiphophostels</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>US$127</t>
+          <t>US$99</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -726,73 +726,73 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>5,517</t>
+          <t>5,885</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hotel The Playce by Happyculture</t>
+          <t>The People - Paris Marais</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>US$450</t>
+          <t>US$159</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2,242</t>
+          <t>6,609</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Le Regent Montmartre by Hiphophostels</t>
+          <t>Hotel des Carmes by Malone</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>US$99</t>
+          <t>US$776</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Exceptional</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5,885</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>citizenM Paris Champs-Élysées</t>
+          <t>Hotel Du Cadran</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>US$1,167</t>
+          <t>US$784</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -807,51 +807,51 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2,787</t>
+          <t>795</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Motel One Paris-Porte Dorée</t>
+          <t>citizenM Paris Champs-Élysées</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>US$495</t>
+          <t>US$1,167</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>6,979</t>
+          <t>2,787</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The People - Paris Bercy</t>
+          <t>Motel One Paris-Porte Dorée</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>US$143</t>
+          <t>US$495</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>8.7</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -861,127 +861,127 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5,976</t>
+          <t>6,979</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>B&amp;B HOTEL Paris 17 Batignolles</t>
+          <t>Beau M Paris</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>US$506</t>
+          <t>US$138</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>8.7</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>12,198</t>
+          <t>1,149</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Beau M Paris</t>
+          <t>The People Paris Belleville</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>US$138</t>
+          <t>US$122</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1,149</t>
+          <t>2,735</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Hôtel Cabane - Orso Hotels</t>
+          <t>Hotel Britannique</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>US$528</t>
+          <t>US$993</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>8.9</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>983</t>
+          <t>1,383</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Hôtel le 209 Paris Bercy</t>
+          <t>Hotel Relais Bosquet by Malone</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>US$547</t>
+          <t>US$924</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>8.7</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3,245</t>
+          <t>1,068</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Hôtel Le Daum</t>
+          <t>Pullman Paris Montparnasse</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>US$536</t>
+          <t>US$1,193</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -996,78 +996,78 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>943</t>
+          <t>2,047</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ibis Paris Gare du Nord Château Landon 10ème</t>
+          <t>Alberte Hôtel</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>US$551</t>
+          <t>US$989</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>9.2</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>4,930</t>
+          <t>169</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Generator Paris</t>
+          <t>Hôtel Oratio</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>US$103</t>
+          <t>US$918</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>9,523</t>
+          <t>1,534</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Elysees Niel Hotel</t>
+          <t>Hôtel Henri IV Rive Gauche</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>US$510</t>
+          <t>US$890</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1077,88 +1077,88 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1,369</t>
+          <t>1,861</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Hôtel Belloy Saint Germain</t>
+          <t>Select Hotel</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>US$776</t>
+          <t>US$884</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Wonderful</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>718</t>
+          <t>2,134</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Hotel Du Cadran</t>
+          <t>Hotel Ekta Champs Elysées</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>US$784</t>
+          <t>US$949</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>8.5</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Very Good</t>
+          <t>Excellent</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>795</t>
+          <t>1,252</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Hotel Monceau Wagram</t>
+          <t>Europe Saint Severin-Paris Notre Dame</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>US$599</t>
+          <t>US$800</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Good</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1,379</t>
+          <t>2,270</t>
         </is>
       </c>
     </row>

</xml_diff>